<commit_message>
v1.6 fix: corrigindo o arquivo -  processar pastas
resolvendo erro de atualização da pasta geral
</commit_message>
<xml_diff>
--- a/log_erros.xlsx
+++ b/log_erros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,160 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24/07/2025 11:59:47</t>
+          <t>24/07/2025 13:29:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CONDONAL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'CONDONAL'.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FOLK</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'FOLK'.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'GA'.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GESTART</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'GESTART'.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HISEG</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'HISEG'.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PRIMEE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'PRIMEE'.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SINGULAR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'SINGULAR'.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>UNICA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'UNICA'.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>VIGON</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Destinatário não encontrado para 'VIGON'.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>24/07/2025 13:29:53</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.7, fix, docs and refactor. Correção do .env, documentação do codigo e refatoração do validador.
fix: correção do arquivo .env de forma que agora os caminhos dos arquivos estao mais seguros no arquivo .env.
docs: adição do readme.txt com a documentação do codigo (explicação de como funciona) e adição de comentarios ao longo do codigo explicando funções para futuras atualizações.
refactor: refatoração do codigo de validação de data na planilha geral.
</commit_message>
<xml_diff>
--- a/log_erros.xlsx
+++ b/log_erros.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:39</t>
+          <t>25/07/2025 10:45:12</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:39</t>
+          <t>25/07/2025 10:45:12</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:39</t>
+          <t>25/07/2025 10:45:12</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:39</t>
+          <t>25/07/2025 10:45:12</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>24/07/2025 13:29:53</t>
+          <t>25/07/2025 10:45:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.8 fix: correção de relatorio do google sheets
corrigindo a falta do contador de arquivo na planilha de relatorio do google sheets
</commit_message>
<xml_diff>
--- a/log_erros.xlsx
+++ b/log_erros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,160 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>25/07/2025 10:45:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CONDONAL</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'CONDONAL'.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FOLK</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'FOLK'.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'GA'.</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:12</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>GESTART</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'GESTART'.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>HISEG</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'HISEG'.</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PRIMEE</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'PRIMEE'.</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SINGULAR</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'SINGULAR'.</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>UNICA</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'UNICA'.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>VIGON</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Destinatário não encontrado para 'VIGON'.</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>25/07/2025 10:45:29</t>
+          <t>25/07/2025 14:58:08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: correção de bugs na data de atualização
</commit_message>
<xml_diff>
--- a/log_erros.xlsx
+++ b/log_erros.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,182 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Destinatário não encontrado.</t>
+          <t>Destinatário não encontrado para 'BASE'.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CONDONAL</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FOLK</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>GERAL</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>GESTART</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>HISEG</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>PRIMEE</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SINGULAR</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>UNICA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>VIGON</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>(-2147221008, 'CoInitialize não foi chamado.', None, None)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>30/07/2025 13:42:01</t>
+          <t>31/07/2025 18:24:35</t>
         </is>
       </c>
     </row>

</xml_diff>